<commit_message>
adding file copy support
</commit_message>
<xml_diff>
--- a/Enterprise_networks.xlsx
+++ b/Enterprise_networks.xlsx
@@ -7,10 +7,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="8436"/>
   </bookViews>
   <sheets>
-    <sheet name="DC_networks" sheetId="10" r:id="rId1"/>
-    <sheet name="Sites_networks" sheetId="11" r:id="rId2"/>
-    <sheet name="Custom_identifier" sheetId="12" r:id="rId3"/>
-    <sheet name="NOT_TO_USE" sheetId="5" r:id="rId4"/>
+    <sheet name="Company_cidr" sheetId="13" r:id="rId1"/>
+    <sheet name="DC_networks" sheetId="10" r:id="rId2"/>
+    <sheet name="Sites_networks" sheetId="11" r:id="rId3"/>
+    <sheet name="Custom_identifier" sheetId="12" r:id="rId4"/>
+    <sheet name="NOT_TO_USE" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Domain">OFFSET(#REF!, 0, 0,COUNT(IF(#REF!="", "", 1)), 1)</definedName>
@@ -26,6 +27,50 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Entire company network range
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>e.g: 10.0.0.0/8</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
@@ -84,7 +129,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
@@ -136,7 +181,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
@@ -176,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="170">
   <si>
     <t>spine</t>
   </si>
@@ -683,13 +728,16 @@
   </si>
   <si>
     <t>Network-Practice-Route</t>
+  </si>
+  <si>
+    <t>Company_network_range</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,6 +765,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1056,11 +1117,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1323,7 +1407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -1351,7 +1435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -1379,7 +1463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E224"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changed j2 templates to supprt apps
</commit_message>
<xml_diff>
--- a/Enterprise_networks.xlsx
+++ b/Enterprise_networks.xlsx
@@ -42,7 +42,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Entire company network range
+          <t xml:space="preserve">Entire company network range, incuding the public space:
 </t>
         </r>
         <r>
@@ -62,7 +62,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+e.g: 21.y.xxxx</t>
         </r>
       </text>
     </comment>
@@ -1119,9 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
updated template to Elastiflow 4.x new data model
</commit_message>
<xml_diff>
--- a/Enterprise_networks.xlsx
+++ b/Enterprise_networks.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F483303-6012-4518-83B4-1B9B0A6CD722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="8436"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company_cidr" sheetId="13" r:id="rId1"/>
@@ -17,22 +18,30 @@
     <definedName name="Domain">OFFSET(#REF!, 0, 0,COUNT(IF(#REF!="", "", 1)), 1)</definedName>
     <definedName name="tenantnames">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -71,12 +80,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -90,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -130,12 +139,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -182,12 +191,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -201,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="175">
   <si>
     <t>spine</t>
   </si>
@@ -731,12 +740,27 @@
   </si>
   <si>
     <t>Company_network_range</t>
+  </si>
+  <si>
+    <t>10.2.20.211</t>
+  </si>
+  <si>
+    <t>10.14.7.0/24</t>
+  </si>
+  <si>
+    <t>10.65.0.8</t>
+  </si>
+  <si>
+    <t>10.100.1.0</t>
+  </si>
+  <si>
+    <t>10.84.35.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1116,10 +1140,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1139,10 +1163,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1406,7 +1430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1434,11 +1458,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,12 +1471,37 @@
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1462,7 +1511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:E224"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">

</xml_diff>